<commit_message>
change Product quantity from fixedpoint to integer
- quantity column in Products sheet of test.xlsx now contains only integers
- quantity is stored as integer in order_lineitems
Jira: LIMS-1936
</commit_message>
<xml_diff>
--- a/bika/lims/setupdata/test/test.xlsx
+++ b/bika/lims/setupdata/test/test.xlsx
@@ -7773,11 +7773,11 @@
   <dataValidations count="6">
     <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Does the client get membership discount?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D8 D10:D14" type="list">
       <formula1>Constants!$G$2:$G$3</formula1>
-      <formula2>0</formula2>
+      <formula2>b</formula2>
     </dataValidation>
     <dataValidation allowBlank="true" operator="equal" prompt="Enter a number and recognised unit separated by a space, e.g. 100 g or 50 ml" promptTitle="Entry format:" showDropDown="false" showErrorMessage="false" showInputMessage="true" sqref="G4:G15" type="none">
       <formula1>0</formula1>
-      <formula2>0</formula2>
+      <formula2>s</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Select a valid entry from the  selction list" errorTitle="Invalid entry" operator="equal" prompt="Select a valid container type from the selection list. The list is maintained on the 'Container Types' sheet" promptTitle="Select a Container Type" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H15" type="list">
       <formula1>'Container Types'!$A$4:$A$102</formula1>
@@ -8077,7 +8077,7 @@
   <dataValidations count="4">
     <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Does the client get membership discount?" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4:G15" type="list">
       <formula1>Constants!$G$2:$G$3</formula1>
-      <formula2>0</formula2>
+      <formula2>u</formula2>
     </dataValidation>
     <dataValidation allowBlank="false" error="Select a valid entry from the drop-down  list of all clients listed on the Clients sheet" errorTitle="Invalid entry" operator="equal" prompt="Select a Client if it is a specific client's private sampling point not available to others. Leave blank if it is a general sampling point that can be used by all clients.  The options on the drop-down list of all clients are maintained on the Clients sheet." promptTitle="Select a valid Client if required" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A15" type="list">
       <formula1>Clients!$A$4:$A$181</formula1>
@@ -17412,7 +17412,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="false" error="Select a valid entry from the drop down list." errorTitle="Invalid Analysis Service" operator="equal" prompt="Select an Analysis Service  from the list. Maintain the list on the 'Analysis Services' sheet" promptTitle="Select an Analysis Service" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A4:A103" type="list">
-      <formula1>'analysis services'!$a$4:$a$141</formula1>
+      <formula1>'Analysis Services'!$A$4:$A$141</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
@@ -26180,7 +26180,7 @@
   <dimension ref="1:12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="H4" activeCellId="0" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -26572,9 +26572,7 @@
       <c r="G10" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="H10" s="100" t="n">
-        <v>1231.5</v>
-      </c>
+      <c r="H10" s="100"/>
       <c r="I10" s="104" t="s">
         <v>950</v>
       </c>
@@ -26707,12 +26705,12 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="greaterThan" prompt="Use . (dot) as delimiter" promptTitle="Quantity in Decimal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H12" type="none">
-      <formula1>0</formula1>
+    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4" type="list">
+      <formula1>Constants!$G$2:$G$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" error="Select 0 or 1  from the drop-down menu" errorTitle="Invalid entry" operator="equal" prompt="Select 1 (True) or 0 (False) from the drop-down menu" promptTitle="Boolean" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G4" type="list">
-      <formula1>Constants!$G$2:$G$3</formula1>
+    <dataValidation allowBlank="true" operator="greaterThan" prompt="Whole number" promptTitle="Quantity" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H4:H12" type="whole">
+      <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>

</xml_diff>